<commit_message>
fix add_row save in xlsx #198 #183
</commit_message>
<xml_diff>
--- a/tests/add_row/has_header_sort_bad.xlsx
+++ b/tests/add_row/has_header_sort_bad.xlsx
@@ -135,14 +135,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B11" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B11">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="b"/>
-        <filter val="ok"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B11"/>
   <tableColumns count="2">
     <tableColumn id="1" name="header1"/>
     <tableColumn id="2" name="header2"/>
@@ -161,7 +154,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -179,11 +172,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -200,7 +193,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
@@ -214,17 +206,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>

</xml_diff>